<commit_message>
commit to my local repository
</commit_message>
<xml_diff>
--- a/data/Connected Office Test Data.xlsx
+++ b/data/Connected Office Test Data.xlsx
@@ -1207,8 +1207,8 @@
       <x:c r="B2" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C2" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D2" s="2" t="b">
         <x:v>0</x:v>
@@ -1224,8 +1224,8 @@
       <x:c r="B3" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C3" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C3" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D3" s="2" t="b">
         <x:v>0</x:v>
@@ -1241,8 +1241,8 @@
       <x:c r="B4" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C4" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C4" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D4" s="2" t="b">
         <x:v>0</x:v>
@@ -1258,8 +1258,8 @@
       <x:c r="B5" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C5" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C5" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D5" s="2" t="b">
         <x:v>0</x:v>
@@ -1275,8 +1275,8 @@
       <x:c r="B6" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C6" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C6" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D6" s="2" t="b">
         <x:v>0</x:v>
@@ -1292,8 +1292,8 @@
       <x:c r="B7" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C7" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C7" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D7" s="2" t="b">
         <x:v>0</x:v>
@@ -1309,8 +1309,8 @@
       <x:c r="B8" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C8" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C8" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D8" s="2" t="b">
         <x:v>0</x:v>
@@ -1326,8 +1326,8 @@
       <x:c r="B9" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C9" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C9" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D9" s="2" t="b">
         <x:v>0</x:v>
@@ -1343,8 +1343,8 @@
       <x:c r="B10" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C10" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C10" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D10" s="2" t="b">
         <x:v>0</x:v>
@@ -1360,8 +1360,8 @@
       <x:c r="B11" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C11" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C11" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D11" s="2" t="b">
         <x:v>0</x:v>
@@ -1377,8 +1377,8 @@
       <x:c r="B12" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C12" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C12" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D12" s="2" t="b">
         <x:v>0</x:v>
@@ -1394,8 +1394,8 @@
       <x:c r="B13" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C13" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C13" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D13" s="2" t="b">
         <x:v>0</x:v>
@@ -1411,8 +1411,8 @@
       <x:c r="B14" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C14" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C14" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D14" s="2" t="b">
         <x:v>0</x:v>
@@ -1428,8 +1428,8 @@
       <x:c r="B15" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C15" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C15" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D15" s="2" t="b">
         <x:v>0</x:v>
@@ -1445,8 +1445,8 @@
       <x:c r="B16" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C16" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C16" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D16" s="2" t="b">
         <x:v>0</x:v>
@@ -1462,8 +1462,8 @@
       <x:c r="B17" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C17" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C17" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D17" s="2" t="b">
         <x:v>0</x:v>
@@ -1479,8 +1479,8 @@
       <x:c r="B18" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C18" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C18" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D18" s="2" t="b">
         <x:v>0</x:v>
@@ -1496,8 +1496,8 @@
       <x:c r="B19" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C19" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C19" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D19" s="2" t="b">
         <x:v>0</x:v>
@@ -1513,8 +1513,8 @@
       <x:c r="B20" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C20" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C20" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D20" s="2" t="b">
         <x:v>0</x:v>
@@ -1530,8 +1530,8 @@
       <x:c r="B21" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C21" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C21" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D21" s="2" t="b">
         <x:v>0</x:v>
@@ -1547,8 +1547,8 @@
       <x:c r="B22" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C22" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C22" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D22" s="2" t="b">
         <x:v>0</x:v>
@@ -1564,8 +1564,8 @@
       <x:c r="B23" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C23" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C23" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D23" s="2" t="b">
         <x:v>0</x:v>
@@ -1581,8 +1581,8 @@
       <x:c r="B24" s="2" t="s">
         <x:v>75</x:v>
       </x:c>
-      <x:c r="C24" s="2" t="b">
-        <x:v>0</x:v>
+      <x:c r="C24" s="2" t="s">
+        <x:v>75</x:v>
       </x:c>
       <x:c r="D24" s="2" t="b">
         <x:v>0</x:v>

</xml_diff>